<commit_message>
update analysis and figures
</commit_message>
<xml_diff>
--- a/worker_data_analysis/workerdata.xlsx
+++ b/worker_data_analysis/workerdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28110" windowHeight="13140"/>
+    <workbookView windowWidth="17500" windowHeight="17160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -226,7 +226,33 @@
     <t>没有</t>
   </si>
   <si>
-    <t>4/1日之后（大概多久）〖60天〗</t>
+    <r>
+      <t>4/1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>日之后（大概多久）〖</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>天〗</t>
+    </r>
   </si>
   <si>
     <t>4/1日之后（大概多久）〖60〗</t>
@@ -643,7 +669,25 @@
     <t>223.104.5.220(上海-上海)</t>
   </si>
   <si>
-    <t>工作机会多┋其他〖工作地近〗</t>
+    <r>
+      <t>工作机会多</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>┋</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他〖工作地近〗</t>
+    </r>
   </si>
   <si>
     <t>21</t>
@@ -1211,6 +1255,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>【无惧无畏】</t>
     </r>
     <r>
@@ -1243,6 +1293,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>高于</t>
     </r>
     <r>
@@ -1271,11 +1327,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1289,7 +1345,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1306,30 +1362,99 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="宋体-简"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1337,30 +1462,28 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -1368,86 +1491,29 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="36">
@@ -1477,7 +1543,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1489,7 +1597,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1501,13 +1627,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1519,7 +1699,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1531,121 +1711,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1671,17 +1737,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1701,20 +1761,28 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1752,266 +1820,239 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="51"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="51" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="51" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="51" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="51" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="51" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="51" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="51" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="51" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="51" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="51" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="51" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="Currency" xfId="12"/>
-    <cellStyle name="已访问的超链接" xfId="13" builtinId="9"/>
-    <cellStyle name="注释" xfId="14" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="15" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="16" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="17" builtinId="11"/>
-    <cellStyle name="标题" xfId="18" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="19" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="20" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="21" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="22" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="23" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="24" builtinId="44"/>
-    <cellStyle name="输出" xfId="25" builtinId="21"/>
-    <cellStyle name="计算" xfId="26" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="27" builtinId="23"/>
-    <cellStyle name="Currency [0]" xfId="28"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="29" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="30" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="31" builtinId="24"/>
-    <cellStyle name="汇总" xfId="32" builtinId="25"/>
-    <cellStyle name="好" xfId="33" builtinId="26"/>
-    <cellStyle name="适中" xfId="34" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="36" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="37" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="38" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="39" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="40" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="41" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="42" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="43" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="44" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="45" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="46" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="47" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="48" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="49" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="50" builtinId="52"/>
-    <cellStyle name="Normal" xfId="51"/>
-    <cellStyle name="Percent" xfId="52"/>
-    <cellStyle name="Comma [0]" xfId="53"/>
-    <cellStyle name="Comma" xfId="54"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2344,11 +2385,11 @@
   <sheetPr/>
   <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="4.14285714285714" customWidth="1"/>
     <col min="2" max="2" width="16.1428571428571" customWidth="1"/>
@@ -2617,7 +2658,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" ht="15" spans="1:26">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -2663,7 +2704,7 @@
       <c r="O4" t="s">
         <v>40</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="17" t="s">
         <v>69</v>
       </c>
       <c r="Q4" t="s">
@@ -3977,7 +4018,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" ht="15" spans="1:26">
       <c r="A21" t="s">
         <v>203</v>
       </c>
@@ -4041,7 +4082,7 @@
       <c r="U21" t="s">
         <v>170</v>
       </c>
-      <c r="V21" t="s">
+      <c r="V21" s="18" t="s">
         <v>208</v>
       </c>
       <c r="W21" t="s">
@@ -5993,9 +6034,9 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="12"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" ht="14.4" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>381</v>
       </c>
@@ -6039,8 +6080,8 @@
       </c>
       <c r="T1" s="9"/>
     </row>
-    <row r="2" ht="12.75" spans="1:20">
-      <c r="A2" s="14">
+    <row r="2" ht="14.4" spans="1:20">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -6052,37 +6093,37 @@
       <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>392</v>
       </c>
       <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="6"/>
       <c r="L2" t="s">
         <v>130</v>
       </c>
       <c r="N2" t="s">
         <v>96</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
       <c r="S2" s="10" t="s">
         <v>275</v>
       </c>
       <c r="T2" s="10"/>
     </row>
-    <row r="3" ht="12.75" spans="1:20">
-      <c r="A3" s="14">
+    <row r="3" spans="1:20">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -6094,19 +6135,19 @@
       <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>392</v>
       </c>
       <c r="H3" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="6"/>
       <c r="L3" t="s">
         <v>159</v>
       </c>
@@ -6123,8 +6164,8 @@
       </c>
       <c r="T3" s="10"/>
     </row>
-    <row r="4" ht="12.75" spans="1:20">
-      <c r="A4" s="14">
+    <row r="4" spans="1:20">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -6136,13 +6177,13 @@
       <c r="E4" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>49</v>
       </c>
       <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="6" t="s">
         <v>185</v>
       </c>
       <c r="J4" s="8" t="s">
@@ -6155,18 +6196,18 @@
       <c r="N4" t="s">
         <v>187</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
       <c r="S4" s="10" t="s">
         <v>246</v>
       </c>
       <c r="T4" s="10"/>
     </row>
-    <row r="5" ht="12.75" spans="1:20">
-      <c r="A5" s="14">
+    <row r="5" ht="14.4" spans="1:20">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -6178,37 +6219,37 @@
       <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>392</v>
       </c>
       <c r="H5" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="6"/>
       <c r="L5" s="1" t="s">
         <v>215</v>
       </c>
       <c r="N5" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
       <c r="S5" s="10">
         <v>18839477910</v>
       </c>
       <c r="T5" s="10"/>
     </row>
-    <row r="6" ht="12.75" spans="1:20">
-      <c r="A6" s="14">
+    <row r="6" spans="1:20">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -6220,37 +6261,37 @@
       <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>392</v>
       </c>
       <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="6"/>
       <c r="L6" t="s">
         <v>186</v>
       </c>
       <c r="N6" t="s">
         <v>187</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
       <c r="S6" s="10" t="s">
         <v>393</v>
       </c>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" ht="12.75" spans="1:20">
-      <c r="A7" s="14">
+    <row r="7" ht="14.4" spans="1:20">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -6262,19 +6303,19 @@
       <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>392</v>
       </c>
       <c r="H7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="K7" s="4"/>
+      <c r="K7" s="6"/>
       <c r="L7" t="s">
         <v>349</v>
       </c>
@@ -6282,18 +6323,18 @@
         <v>107</v>
       </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="3" t="s">
+      <c r="P7" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
       <c r="S7" s="10" t="s">
         <v>351</v>
       </c>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" ht="12.75" spans="1:20">
-      <c r="A8" s="14">
+    <row r="8" spans="1:20">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -6305,7 +6346,7 @@
       <c r="E8" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>49</v>
       </c>
       <c r="H8" t="s">
@@ -6331,8 +6372,8 @@
       </c>
       <c r="T8" s="10"/>
     </row>
-    <row r="9" ht="12.75" spans="1:20">
-      <c r="A9" s="14">
+    <row r="9" ht="14.4" spans="1:20">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -6344,7 +6385,7 @@
       <c r="E9" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="14" t="s">
         <v>392</v>
       </c>
       <c r="H9" t="s">
@@ -6362,18 +6403,18 @@
       <c r="N9" t="s">
         <v>100</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="P9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
       <c r="S9" s="10" t="s">
         <v>161</v>
       </c>
       <c r="T9" s="10"/>
     </row>
-    <row r="10" ht="12.75" spans="1:20">
-      <c r="A10" s="14">
+    <row r="10" spans="1:20">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -6385,7 +6426,7 @@
       <c r="E10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>392</v>
       </c>
       <c r="H10" t="s">
@@ -6413,8 +6454,8 @@
       </c>
       <c r="T10" s="10"/>
     </row>
-    <row r="11" ht="12.75" spans="1:20">
-      <c r="A11" s="14">
+    <row r="11" spans="1:20">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -6426,7 +6467,7 @@
       <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>392</v>
       </c>
       <c r="H11" t="s">
@@ -6452,23 +6493,23 @@
       </c>
       <c r="T11" s="10"/>
     </row>
-    <row r="12" ht="12.75" spans="1:1">
-      <c r="A12" s="14"/>
+    <row r="12" spans="1:1">
+      <c r="A12" s="13"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="14"/>
+      <c r="A15" s="13"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="14"/>
+      <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="77">
@@ -6558,15 +6599,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="12" outlineLevelRow="6"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" ht="14.4" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>381</v>
       </c>
@@ -6610,7 +6651,7 @@
       </c>
       <c r="T1" s="9"/>
     </row>
-    <row r="2" ht="12.75" spans="1:20">
+    <row r="2" ht="14.4" spans="1:20">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6623,7 +6664,7 @@
       <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>394</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -6643,17 +6684,17 @@
         <v>35</v>
       </c>
       <c r="O2" s="1"/>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
       <c r="S2" s="10" t="s">
         <v>333</v>
       </c>
       <c r="T2" s="10"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" ht="14.4" spans="1:20">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6666,7 +6707,7 @@
       <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>394</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -6695,42 +6736,42 @@
       </c>
       <c r="T3" s="10"/>
     </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="5">
+    <row r="4" ht="15" spans="1:20">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="6" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6" t="s">
+      <c r="M4" s="3"/>
+      <c r="N4" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="O4" s="5"/>
+      <c r="O4" s="3"/>
       <c r="P4" s="7" t="s">
         <v>74</v>
       </c>
@@ -6739,9 +6780,9 @@
       <c r="S4" s="12" t="s">
         <v>365</v>
       </c>
-      <c r="T4" s="13"/>
+      <c r="T4" s="12"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" ht="14.4" spans="1:20">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6754,7 +6795,7 @@
       <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="5" t="s">
         <v>394</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -6772,17 +6813,17 @@
       <c r="N5" t="s">
         <v>187</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
       <c r="S5" s="10" t="s">
         <v>309</v>
       </c>
       <c r="T5" s="10"/>
     </row>
-    <row r="6" ht="12.75" spans="1:20">
+    <row r="6" ht="14.4" spans="1:20">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6795,7 +6836,7 @@
       <c r="E6" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="5" t="s">
         <v>394</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -6821,7 +6862,7 @@
       </c>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" ht="12.75" spans="1:20">
+    <row r="7" ht="14.4" spans="1:20">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6834,7 +6875,7 @@
       <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="5" t="s">
         <v>394</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -6862,9 +6903,6 @@
       </c>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" ht="12.75"/>
-    <row r="10" ht="12.75"/>
-    <row r="13" ht="12.75"/>
   </sheetData>
   <mergeCells count="49">
     <mergeCell ref="B1:C1"/>

</xml_diff>